<commit_message>
Sesuailkan colum, ringkas code, contoh ekspor
</commit_message>
<xml_diff>
--- a/assets/import/contoh_penduduk.xlsx
+++ b/assets/import/contoh_penduduk.xlsx
@@ -335,7 +335,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ2" s="0" t="inlineStr">
+      <c r="AK2" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -437,7 +437,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ3" s="0" t="inlineStr">
+      <c r="AK3" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -539,7 +539,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ4" s="0" t="inlineStr">
+      <c r="AK4" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -641,7 +641,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ5" s="0" t="inlineStr">
+      <c r="AK5" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -743,7 +743,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ6" s="0" t="inlineStr">
+      <c r="AK6" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -845,7 +845,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ7" s="0" t="inlineStr">
+      <c r="AK7" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -947,7 +947,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ8" s="0" t="inlineStr">
+      <c r="AK8" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1049,7 +1049,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ9" s="0" t="inlineStr">
+      <c r="AK9" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1151,7 +1151,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ10" s="0" t="inlineStr">
+      <c r="AK10" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1253,7 +1253,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ11" s="0" t="inlineStr">
+      <c r="AK11" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1355,7 +1355,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ12" s="0" t="inlineStr">
+      <c r="AK12" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1457,7 +1457,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ13" s="0" t="inlineStr">
+      <c r="AK13" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1559,7 +1559,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ14" s="0" t="inlineStr">
+      <c r="AK14" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1661,7 +1661,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ15" s="0" t="inlineStr">
+      <c r="AK15" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1763,7 +1763,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ16" s="0" t="inlineStr">
+      <c r="AK16" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1865,7 +1865,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ17" s="0" t="inlineStr">
+      <c r="AK17" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1967,7 +1967,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ18" s="0" t="inlineStr">
+      <c r="AK18" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -2069,7 +2069,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ19" s="0" t="inlineStr">
+      <c r="AK19" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -2171,7 +2171,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ20" s="0" t="inlineStr">
+      <c r="AK20" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -2273,7 +2273,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ21" s="0" t="inlineStr">
+      <c r="AK21" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -2375,7 +2375,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ22" s="0" t="inlineStr">
+      <c r="AK22" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -2477,7 +2477,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ23" s="0" t="inlineStr">
+      <c r="AK23" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -2579,7 +2579,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ24" s="0" t="inlineStr">
+      <c r="AK24" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -2681,7 +2681,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ25" s="0" t="inlineStr">
+      <c r="AK25" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -2783,7 +2783,7 @@
           <t>2</t>
         </is>
       </c>
-      <c r="AJ26" s="0" t="inlineStr">
+      <c r="AK26" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -2885,7 +2885,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ27" s="0" t="inlineStr">
+      <c r="AK27" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -2987,7 +2987,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ28" s="0" t="inlineStr">
+      <c r="AK28" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -3089,7 +3089,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ29" s="0" t="inlineStr">
+      <c r="AK29" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -3191,7 +3191,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ30" s="0" t="inlineStr">
+      <c r="AK30" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -3293,7 +3293,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ31" s="0" t="inlineStr">
+      <c r="AK31" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -3395,7 +3395,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ32" s="0" t="inlineStr">
+      <c r="AK32" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -3497,7 +3497,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ33" s="0" t="inlineStr">
+      <c r="AK33" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -3599,7 +3599,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ34" s="0" t="inlineStr">
+      <c r="AK34" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -3701,7 +3701,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ35" s="0" t="inlineStr">
+      <c r="AK35" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -3803,7 +3803,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ36" s="0" t="inlineStr">
+      <c r="AK36" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -3905,7 +3905,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ37" s="0" t="inlineStr">
+      <c r="AK37" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -4007,7 +4007,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ38" s="0" t="inlineStr">
+      <c r="AK38" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -4109,7 +4109,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ39" s="0" t="inlineStr">
+      <c r="AK39" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -4211,7 +4211,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ40" s="0" t="inlineStr">
+      <c r="AK40" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -4313,7 +4313,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ41" s="0" t="inlineStr">
+      <c r="AK41" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -4415,7 +4415,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ42" s="0" t="inlineStr">
+      <c r="AK42" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -4517,7 +4517,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ43" s="0" t="inlineStr">
+      <c r="AK43" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -4619,7 +4619,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ44" s="0" t="inlineStr">
+      <c r="AK44" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -4721,7 +4721,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ45" s="0" t="inlineStr">
+      <c r="AK45" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -4823,7 +4823,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ46" s="0" t="inlineStr">
+      <c r="AK46" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -4925,7 +4925,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ47" s="0" t="inlineStr">
+      <c r="AK47" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -5027,7 +5027,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ48" s="0" t="inlineStr">
+      <c r="AK48" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -5129,7 +5129,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ49" s="0" t="inlineStr">
+      <c r="AK49" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -5231,7 +5231,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ50" s="0" t="inlineStr">
+      <c r="AK50" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -5333,7 +5333,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ51" s="0" t="inlineStr">
+      <c r="AK51" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -5435,7 +5435,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ52" s="0" t="inlineStr">
+      <c r="AK52" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -5537,7 +5537,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ53" s="0" t="inlineStr">
+      <c r="AK53" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -5639,7 +5639,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ54" s="0" t="inlineStr">
+      <c r="AK54" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -5741,7 +5741,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ55" s="0" t="inlineStr">
+      <c r="AK55" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -5843,7 +5843,7 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AJ56" s="0" t="inlineStr">
+      <c r="AK56" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -5945,7 +5945,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ57" s="0" t="inlineStr">
+      <c r="AK57" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -6047,7 +6047,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ58" s="0" t="inlineStr">
+      <c r="AK58" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -6149,7 +6149,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ59" s="0" t="inlineStr">
+      <c r="AK59" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -6251,7 +6251,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ60" s="0" t="inlineStr">
+      <c r="AK60" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -6353,7 +6353,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ61" s="0" t="inlineStr">
+      <c r="AK61" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -6455,7 +6455,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ62" s="0" t="inlineStr">
+      <c r="AK62" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -6557,7 +6557,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ63" s="0" t="inlineStr">
+      <c r="AK63" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -6659,7 +6659,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ64" s="0" t="inlineStr">
+      <c r="AK64" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -6761,7 +6761,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ65" s="0" t="inlineStr">
+      <c r="AK65" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -6863,7 +6863,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ66" s="0" t="inlineStr">
+      <c r="AK66" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -6965,7 +6965,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ67" s="0" t="inlineStr">
+      <c r="AK67" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -7067,7 +7067,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ68" s="0" t="inlineStr">
+      <c r="AK68" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -7169,7 +7169,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ69" s="0" t="inlineStr">
+      <c r="AK69" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -7271,7 +7271,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ70" s="0" t="inlineStr">
+      <c r="AK70" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -7373,7 +7373,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ71" s="0" t="inlineStr">
+      <c r="AK71" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -7475,7 +7475,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ72" s="0" t="inlineStr">
+      <c r="AK72" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -7577,7 +7577,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ73" s="0" t="inlineStr">
+      <c r="AK73" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -7679,7 +7679,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ74" s="0" t="inlineStr">
+      <c r="AK74" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -7781,7 +7781,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ75" s="0" t="inlineStr">
+      <c r="AK75" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -7883,7 +7883,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ76" s="0" t="inlineStr">
+      <c r="AK76" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -7985,7 +7985,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ77" s="0" t="inlineStr">
+      <c r="AK77" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -8087,7 +8087,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ78" s="0" t="inlineStr">
+      <c r="AK78" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -8189,7 +8189,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ79" s="0" t="inlineStr">
+      <c r="AK79" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -8291,7 +8291,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ80" s="0" t="inlineStr">
+      <c r="AK80" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -8393,7 +8393,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ81" s="0" t="inlineStr">
+      <c r="AK81" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -8495,7 +8495,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ82" s="0" t="inlineStr">
+      <c r="AK82" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -8597,7 +8597,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ83" s="0" t="inlineStr">
+      <c r="AK83" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -8699,7 +8699,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ84" s="0" t="inlineStr">
+      <c r="AK84" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -8801,7 +8801,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ85" s="0" t="inlineStr">
+      <c r="AK85" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -8903,7 +8903,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ86" s="0" t="inlineStr">
+      <c r="AK86" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -9005,7 +9005,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ87" s="0" t="inlineStr">
+      <c r="AK87" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -9107,7 +9107,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ88" s="0" t="inlineStr">
+      <c r="AK88" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -9209,7 +9209,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ89" s="0" t="inlineStr">
+      <c r="AK89" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -9311,7 +9311,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ90" s="0" t="inlineStr">
+      <c r="AK90" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -9413,7 +9413,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ91" s="0" t="inlineStr">
+      <c r="AK91" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -9515,7 +9515,7 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AJ92" s="0" t="inlineStr">
+      <c r="AK92" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -9617,7 +9617,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ93" s="0" t="inlineStr">
+      <c r="AK93" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -9719,7 +9719,7 @@
           <t>2</t>
         </is>
       </c>
-      <c r="AJ94" s="0" t="inlineStr">
+      <c r="AK94" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -9821,7 +9821,7 @@
           <t>5</t>
         </is>
       </c>
-      <c r="AJ95" s="0" t="inlineStr">
+      <c r="AK95" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -9923,7 +9923,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ96" s="0" t="inlineStr">
+      <c r="AK96" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -10025,7 +10025,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ97" s="0" t="inlineStr">
+      <c r="AK97" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -10127,7 +10127,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="AJ98" s="0" t="inlineStr">
+      <c r="AK98" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>

</xml_diff>

<commit_message>
Gabungkan rilis premium 2306.0.3-clear
</commit_message>
<xml_diff>
--- a/assets/import/contoh_penduduk.xlsx
+++ b/assets/import/contoh_penduduk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\open-desa\premium\assets\import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT OPENDESA\OpenSID\assets\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F8BC1A-4420-4370-B97B-196FCC227883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D1560B-6567-4E6D-BB5D-7A587BD93687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1624,10 +1624,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1845,8 +1844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J50" workbookViewId="0">
-      <selection activeCell="R57" sqref="R57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1855,127 +1854,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>481</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>482</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>483</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>484</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>485</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>486</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>487</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s">
         <v>488</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s">
         <v>489</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" t="s">
         <v>490</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" t="s">
         <v>491</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" t="s">
         <v>492</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" t="s">
         <v>493</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" t="s">
         <v>494</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" t="s">
         <v>495</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" t="s">
         <v>496</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" t="s">
         <v>497</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" t="s">
         <v>498</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" t="s">
         <v>499</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" t="s">
         <v>500</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" t="s">
         <v>501</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" t="s">
         <v>502</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" t="s">
         <v>503</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" t="s">
         <v>504</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" t="s">
         <v>505</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" t="s">
         <v>506</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" t="s">
         <v>507</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" t="s">
         <v>508</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" t="s">
         <v>509</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" t="s">
         <v>510</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AE1" t="s">
         <v>511</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AF1" t="s">
         <v>512</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AG1" t="s">
         <v>513</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AH1" t="s">
         <v>514</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AI1" t="s">
         <v>515</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AJ1" t="s">
         <v>516</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AK1" t="s">
         <v>517</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AL1" t="s">
         <v>518</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AM1" t="s">
         <v>519</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AN1" t="s">
         <v>520</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AO1" t="s">
         <v>521</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Persiapan rilis umum v2312.1.0 (#7531)
</commit_message>
<xml_diff>
--- a/assets/import/contoh_penduduk.xlsx
+++ b/assets/import/contoh_penduduk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\open-desa\premium\assets\import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT OPENDESA\OpenSID\assets\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F8BC1A-4420-4370-B97B-196FCC227883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D1560B-6567-4E6D-BB5D-7A587BD93687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1624,10 +1624,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1845,8 +1844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J50" workbookViewId="0">
-      <selection activeCell="R57" sqref="R57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1855,127 +1854,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>481</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>482</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>483</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>484</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>485</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>486</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>487</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s">
         <v>488</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s">
         <v>489</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" t="s">
         <v>490</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" t="s">
         <v>491</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" t="s">
         <v>492</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" t="s">
         <v>493</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" t="s">
         <v>494</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" t="s">
         <v>495</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" t="s">
         <v>496</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" t="s">
         <v>497</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" t="s">
         <v>498</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" t="s">
         <v>499</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" t="s">
         <v>500</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" t="s">
         <v>501</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" t="s">
         <v>502</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" t="s">
         <v>503</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" t="s">
         <v>504</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" t="s">
         <v>505</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" t="s">
         <v>506</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" t="s">
         <v>507</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" t="s">
         <v>508</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" t="s">
         <v>509</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" t="s">
         <v>510</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AE1" t="s">
         <v>511</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AF1" t="s">
         <v>512</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AG1" t="s">
         <v>513</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AH1" t="s">
         <v>514</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AI1" t="s">
         <v>515</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AJ1" t="s">
         <v>516</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AK1" t="s">
         <v>517</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AL1" t="s">
         <v>518</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AM1" t="s">
         <v>519</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AN1" t="s">
         <v>520</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AO1" t="s">
         <v>521</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WIP: Ekspor dan Impor Data Koordinat (Lat, Lng) Penduduk
</commit_message>
<xml_diff>
--- a/assets/import/contoh_penduduk.xlsx
+++ b/assets/import/contoh_penduduk.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT OPENDESA\OpenSID\assets\import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon-6.0.0\www\Desaku\assets\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D1560B-6567-4E6D-BB5D-7A587BD93687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4067203D-D2CB-4E2D-AB72-15218B92A35C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1981" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1983" uniqueCount="524">
   <si>
     <t>MANGSIT</t>
   </si>
@@ -1586,6 +1586,12 @@
   </si>
   <si>
     <t>no_asuransi</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>lng</t>
   </si>
 </sst>
 </file>
@@ -1624,9 +1630,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1842,18 +1849,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO1000"/>
+  <dimension ref="A1:AQ1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AP6" sqref="AP6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="39" width="8.5" customWidth="1"/>
+    <col min="42" max="42" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="20.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>481</v>
       </c>
@@ -1977,8 +1986,14 @@
       <c r="AO1" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="2" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AP1" t="s">
+        <v>522</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2039,8 +2054,14 @@
       <c r="AK2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AP2">
+        <v>1</v>
+      </c>
+      <c r="AQ2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2101,8 +2122,14 @@
       <c r="AK3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AP3" s="2">
+        <v>-8495339739996280</v>
+      </c>
+      <c r="AQ3" s="2">
+        <v>1.1605342939496E+16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2164,7 +2191,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2226,7 +2253,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
@@ -2288,7 +2315,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
@@ -2350,7 +2377,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
@@ -2412,7 +2439,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>26</v>
       </c>
@@ -2474,7 +2501,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>51</v>
       </c>
@@ -2536,7 +2563,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>51</v>
       </c>
@@ -2598,7 +2625,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>51</v>
       </c>
@@ -2660,7 +2687,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>68</v>
       </c>
@@ -2722,7 +2749,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>68</v>
       </c>
@@ -2784,7 +2811,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>68</v>
       </c>
@@ -2846,7 +2873,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>68</v>
       </c>

</xml_diff>